<commit_message>
Correción de tiempos set up archivo excel y visio
</commit_message>
<xml_diff>
--- a/SimulacionProceso/Tiempos por proceso.xlsx
+++ b/SimulacionProceso/Tiempos por proceso.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/miarodriguezur_unal_edu_co/Documents/Doceabo semestre/AUTO/proyecto Auto/Proyecto_APM/SimulacionProceso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{61B3FD6E-7C42-47FA-BDD5-3422E8C15841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{498A6CE1-0065-47E4-9DFF-ABA2920049A5}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{0EE92507-21CF-4F82-8EBE-D3C7CE82A09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{4CA7F2C6-3765-4F42-B624-D8E8E0157753}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8728B57-2FEA-4814-B387-671D8068A2D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C8728B57-2FEA-4814-B387-671D8068A2D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t>Corte</t>
   </si>
@@ -137,9 +138,6 @@
     <t>ETAPAS</t>
   </si>
   <si>
-    <t>Tiempo Operativo (Minutos)</t>
-  </si>
-  <si>
     <t>Tiempo Estandar (Minutos)</t>
   </si>
   <si>
@@ -150,6 +148,21 @@
   </si>
   <si>
     <t>Set-up time</t>
+  </si>
+  <si>
+    <t>Tiempo Operativo + Setup (Minutos)</t>
+  </si>
+  <si>
+    <t>Tiempo Proceso (HH:MM:SS)</t>
+  </si>
+  <si>
+    <t>Tiempo Operativo + Setup (HH:MM:SS)</t>
+  </si>
+  <si>
+    <t>Set-up time (HH:MM:SS)</t>
+  </si>
+  <si>
+    <t>Tiempo Proceso (Segundos)</t>
   </si>
 </sst>
 </file>
@@ -173,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +202,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,40 +239,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,6 +263,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95354742-4944-432B-9318-6015475B4974}">
   <dimension ref="B6:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,729 +634,729 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="I6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="K6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="13">
+      <c r="F7" s="14"/>
+      <c r="G7" s="5">
         <v>3.75</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="5">
         <v>4.32</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="10">
         <f>G7/1440</f>
         <v>2.6041666666666665E-3</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="10">
         <f>H7/1440</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="10">
         <f>J7-I7</f>
         <v>3.9583333333333354E-4</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="13">
+      <c r="F8" s="14"/>
+      <c r="G8" s="5">
         <v>4.12</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="5">
         <v>4.75</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="10">
         <f t="shared" ref="I8:I30" si="0">G8/1440</f>
         <v>2.8611111111111111E-3</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="10">
         <f t="shared" ref="J8:J30" si="1">H8/1440</f>
         <v>3.2986111111111111E-3</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="10">
         <f t="shared" ref="K8:K30" si="2">J8-I8</f>
         <v>4.3749999999999995E-4</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="13">
+      <c r="F9" s="14"/>
+      <c r="G9" s="5">
         <v>1.2</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="5">
         <v>1.4</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>8.3333333333333328E-4</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>9.7222222222222219E-4</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="10">
         <f t="shared" si="2"/>
         <v>1.3888888888888892E-4</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="4">
+      <c r="B10" s="11"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="5">
         <v>2.67</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="5">
         <v>3.06</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="10">
         <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="10">
         <f t="shared" si="2"/>
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="5">
         <v>2.67</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="5">
         <v>3.06</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="10">
         <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="10">
         <f t="shared" si="2"/>
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="5">
         <v>2.67</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="5">
         <v>3.06</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="10">
         <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="10">
         <f t="shared" si="2"/>
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="13">
+      <c r="F13" s="14"/>
+      <c r="G13" s="5">
         <v>9.4</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="5">
         <v>10.81</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="10">
         <f t="shared" si="0"/>
         <v>6.5277777777777782E-3</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>7.5069444444444446E-3</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="10">
         <f t="shared" si="2"/>
         <v>9.7916666666666638E-4</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="13">
+      <c r="F14" s="14"/>
+      <c r="G14" s="5">
         <v>0.24</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="5">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="10">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>1.9444444444444446E-4</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="10">
         <f t="shared" si="2"/>
         <v>2.7777777777777799E-5</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2">
         <v>7</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13">
+      <c r="F15" s="14"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
         <v>1.97</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
         <v>1.3680555555555555E-3</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="10">
         <f t="shared" si="2"/>
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="2">
         <v>8</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13">
+      <c r="F16" s="14"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
         <v>1.97</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="10">
         <f t="shared" si="1"/>
         <v>1.3680555555555555E-3</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="10">
         <f t="shared" si="2"/>
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="2">
         <v>9</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="13">
+      <c r="F17" s="14"/>
+      <c r="G17" s="5">
         <v>4.96</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="5">
         <v>5.7</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="10">
         <f t="shared" si="0"/>
         <v>3.4444444444444444E-3</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="10">
         <f t="shared" si="1"/>
         <v>3.9583333333333337E-3</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="10">
         <f t="shared" si="2"/>
         <v>5.1388888888888925E-4</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="2">
         <v>10</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13">
+      <c r="F18" s="14"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5">
         <v>1.97</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="10">
         <f t="shared" si="1"/>
         <v>1.3680555555555555E-3</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="10">
         <f t="shared" si="2"/>
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>11</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="13">
+      <c r="F19" s="18"/>
+      <c r="G19" s="5">
         <v>0.44</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="5">
         <v>0.5</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="10">
         <f t="shared" si="0"/>
         <v>3.0555555555555555E-4</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="10">
         <f t="shared" si="1"/>
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="10">
         <f t="shared" si="2"/>
         <v>4.1666666666666686E-5</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="7">
+      <c r="B20" s="12"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="4">
         <v>12</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="13">
+      <c r="F20" s="18"/>
+      <c r="G20" s="5">
         <v>1.97</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="5">
         <v>2.2599999999999998</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="10">
         <f t="shared" si="0"/>
         <v>1.3680555555555555E-3</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="10">
         <f t="shared" si="1"/>
         <v>1.5694444444444443E-3</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="10">
         <f t="shared" si="2"/>
         <v>2.0138888888888875E-4</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="7">
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="4">
         <v>13</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="13">
+      <c r="F21" s="18"/>
+      <c r="G21" s="5">
         <v>1.26</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="5">
         <v>1.45</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="10">
         <f t="shared" si="0"/>
         <v>8.7500000000000002E-4</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="10">
         <f t="shared" si="1"/>
         <v>1.0069444444444444E-3</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="10">
         <f t="shared" si="2"/>
         <v>1.3194444444444441E-4</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="7">
+      <c r="B22" s="12"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="4">
         <v>15</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="13">
+      <c r="F22" s="18"/>
+      <c r="G22" s="5">
         <v>0.95</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="10">
         <f t="shared" si="0"/>
         <v>6.5972222222222224E-4</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="10">
         <f t="shared" si="1"/>
         <v>7.6388888888888893E-4</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="10">
         <f t="shared" si="2"/>
         <v>1.0416666666666669E-4</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="7">
+      <c r="B23" s="12"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="4">
         <v>16</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="13">
+      <c r="F23" s="18"/>
+      <c r="G23" s="5">
         <v>4.26</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="10">
         <f t="shared" si="0"/>
         <v>2.9583333333333332E-3</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="10">
         <f t="shared" si="1"/>
         <v>3.402777777777778E-3</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K23" s="10">
         <f t="shared" si="2"/>
         <v>4.4444444444444479E-4</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="7">
+      <c r="B24" s="12"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="4">
         <v>17</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="13">
+      <c r="F24" s="18"/>
+      <c r="G24" s="5">
         <v>4.29</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="5">
         <v>4.93</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="10">
         <f t="shared" si="0"/>
         <v>2.9791666666666669E-3</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="10">
         <f t="shared" si="1"/>
         <v>3.4236111111111108E-3</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="10">
         <f t="shared" si="2"/>
         <v>4.4444444444444392E-4</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>18</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="13">
+      <c r="F25" s="18"/>
+      <c r="G25" s="5">
         <v>3.59</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="5">
         <v>4.13</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="10">
         <f t="shared" si="0"/>
         <v>2.4930555555555556E-3</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="10">
         <f t="shared" si="1"/>
         <v>2.8680555555555555E-3</v>
       </c>
-      <c r="K25" s="18">
+      <c r="K25" s="10">
         <f t="shared" si="2"/>
         <v>3.749999999999999E-4</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="7">
+      <c r="B26" s="12"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="4">
         <v>19</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="13">
+      <c r="F26" s="18"/>
+      <c r="G26" s="5">
         <v>2.39</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="5">
         <v>2.76</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="10">
         <f t="shared" si="0"/>
         <v>1.6597222222222224E-3</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="10">
         <f t="shared" si="1"/>
         <v>1.9166666666666666E-3</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="10">
         <f t="shared" si="2"/>
         <v>2.5694444444444419E-4</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="7">
+      <c r="B27" s="12"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="4">
         <v>22</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="13">
+      <c r="F27" s="18"/>
+      <c r="G27" s="5">
         <v>4.16</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="5">
         <v>4.8</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="10">
         <f t="shared" si="0"/>
         <v>2.8888888888888892E-3</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="10">
         <f t="shared" si="1"/>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="10">
         <f t="shared" si="2"/>
         <v>4.4444444444444392E-4</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>14</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="13">
+      <c r="F28" s="18"/>
+      <c r="G28" s="5">
         <v>3.48</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="5">
         <v>4</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="10">
         <f t="shared" si="0"/>
         <v>2.4166666666666668E-3</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="10">
         <f t="shared" si="1"/>
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="10">
         <f t="shared" si="2"/>
         <v>3.6111111111111109E-4</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="7">
+      <c r="B29" s="12"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="4">
         <v>20</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="13">
+      <c r="F29" s="18"/>
+      <c r="G29" s="5">
         <v>1.03</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="5">
         <v>1.2</v>
       </c>
-      <c r="I29" s="18">
+      <c r="I29" s="10">
         <f t="shared" si="0"/>
         <v>7.1527777777777779E-4</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="10">
         <f t="shared" si="1"/>
         <v>8.3333333333333328E-4</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="10">
         <f t="shared" si="2"/>
         <v>1.1805555555555549E-4</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="7">
+      <c r="B30" s="12"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="4">
         <v>21</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="13">
+      <c r="F30" s="18"/>
+      <c r="G30" s="5">
         <v>0.49</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H30" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="10">
         <f t="shared" si="0"/>
         <v>3.4027777777777778E-4</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="10">
         <f t="shared" si="1"/>
         <v>3.9583333333333332E-4</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="10">
         <f t="shared" si="2"/>
         <v>5.5555555555555545E-5</v>
       </c>
@@ -1343,6 +1374,10 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="B7:B18"/>
     <mergeCell ref="B19:B30"/>
     <mergeCell ref="D10:D12"/>
@@ -1359,11 +1394,1216 @@
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="C28:C30"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A6CFB2-59B8-49B2-A007-7D9BE44E8259}">
+  <dimension ref="B3:Q27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="5">
+        <v>3.75</v>
+      </c>
+      <c r="H4" s="5">
+        <v>4.32</v>
+      </c>
+      <c r="I4" s="5">
+        <v>60</v>
+      </c>
+      <c r="J4" s="10">
+        <f>G4/1440</f>
+        <v>2.6041666666666665E-3</v>
+      </c>
+      <c r="K4" s="10">
+        <f>H4/1440</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L4" s="24">
+        <f>I4/86400</f>
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M4" s="24">
+        <f>K4-L4</f>
+        <v>2.3055555555555555E-3</v>
+      </c>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="5">
+        <v>4.12</v>
+      </c>
+      <c r="H5" s="5">
+        <v>4.75</v>
+      </c>
+      <c r="I5" s="5">
+        <v>80</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" ref="J5:J27" si="0">G5/1440</f>
+        <v>2.8611111111111111E-3</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" ref="K5:K27" si="1">H5/1440</f>
+        <v>3.2986111111111111E-3</v>
+      </c>
+      <c r="L5" s="24">
+        <f t="shared" ref="L5:L27" si="2">I5/86400</f>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="M5" s="24">
+        <f t="shared" ref="M5:M27" si="3">K5-L5</f>
+        <v>2.3726851851851851E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="I6" s="5">
+        <v>24</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333328E-4</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="1"/>
+        <v>9.7222222222222219E-4</v>
+      </c>
+      <c r="L6" s="24">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777778E-4</v>
+      </c>
+      <c r="M6" s="24">
+        <f t="shared" si="3"/>
+        <v>6.9444444444444436E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13">
+        <v>4</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2.67</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.06</v>
+      </c>
+      <c r="I7" s="5">
+        <v>69</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8541666666666667E-3</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="1"/>
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="L7" s="24">
+        <f t="shared" si="2"/>
+        <v>7.9861111111111116E-4</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="3"/>
+        <v>1.3263888888888891E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2.67</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3.06</v>
+      </c>
+      <c r="I8" s="5">
+        <v>35</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8541666666666667E-3</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="1"/>
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="L8" s="24">
+        <f t="shared" si="2"/>
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="M8" s="24">
+        <f t="shared" si="3"/>
+        <v>1.7199074074074076E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2.67</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3.06</v>
+      </c>
+      <c r="I9" s="5">
+        <v>20</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8541666666666667E-3</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="1"/>
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="L9" s="24">
+        <f t="shared" si="2"/>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="M9" s="24">
+        <f t="shared" si="3"/>
+        <v>1.8935185185185188E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="5">
+        <v>9.4</v>
+      </c>
+      <c r="H10" s="5">
+        <v>10.81</v>
+      </c>
+      <c r="I10" s="5">
+        <v>300</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="0"/>
+        <v>6.5277777777777782E-3</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="1"/>
+        <v>7.5069444444444446E-3</v>
+      </c>
+      <c r="L10" s="24">
+        <f t="shared" si="2"/>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M10" s="24">
+        <f t="shared" si="3"/>
+        <v>4.0347222222222225E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="5">
+        <v>0.24</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I11" s="5">
+        <v>4</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="K11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9444444444444446E-4</v>
+      </c>
+      <c r="L11" s="24">
+        <f t="shared" si="2"/>
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="M11" s="24">
+        <f t="shared" si="3"/>
+        <v>1.4814814814814817E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="I12" s="5">
+        <v>207</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="L12" s="24">
+        <f t="shared" si="2"/>
+        <v>2.3958333333333331E-3</v>
+      </c>
+      <c r="M12" s="24">
+        <f t="shared" si="3"/>
+        <v>3.4722222222222446E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="I13" s="5">
+        <v>71</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="1"/>
+        <v>8.4027777777777779E-4</v>
+      </c>
+      <c r="L13" s="24">
+        <f t="shared" si="2"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="M13" s="24">
+        <f t="shared" si="3"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="2">
+        <v>9</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="5">
+        <v>4.96</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5.7</v>
+      </c>
+      <c r="I14" s="5">
+        <v>270</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="0"/>
+        <v>3.4444444444444444E-3</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="1"/>
+        <v>3.9583333333333337E-3</v>
+      </c>
+      <c r="L14" s="24">
+        <f t="shared" si="2"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="M14" s="24">
+        <f t="shared" si="3"/>
+        <v>8.333333333333335E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="2">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>1.21</v>
+      </c>
+      <c r="I15" s="5">
+        <v>71</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="1"/>
+        <v>8.4027777777777779E-4</v>
+      </c>
+      <c r="L15" s="24">
+        <f t="shared" si="2"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="M15" s="24">
+        <f t="shared" si="3"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4">
+        <v>11</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="5">
+        <v>20</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="0"/>
+        <v>3.0555555555555555E-4</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="L16" s="24">
+        <f t="shared" si="2"/>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="M16" s="24">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="4">
+        <v>12</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="5">
+        <v>1.97</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I17" s="5">
+        <v>100</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="0"/>
+        <v>1.3680555555555555E-3</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5694444444444443E-3</v>
+      </c>
+      <c r="L17" s="24">
+        <f t="shared" si="2"/>
+        <v>1.1574074074074073E-3</v>
+      </c>
+      <c r="M17" s="24">
+        <f t="shared" si="3"/>
+        <v>4.1203703703703693E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="4">
+        <v>13</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="I18" s="5">
+        <v>80</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="0"/>
+        <v>8.7500000000000002E-4</v>
+      </c>
+      <c r="K18" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0069444444444444E-3</v>
+      </c>
+      <c r="L18" s="24">
+        <f t="shared" si="2"/>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="M18" s="24">
+        <f t="shared" si="3"/>
+        <v>8.1018518518518462E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="4">
+        <v>15</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I19" s="5">
+        <v>60</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="0"/>
+        <v>6.5972222222222224E-4</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="1"/>
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="L19" s="24">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M19" s="24">
+        <f t="shared" si="3"/>
+        <v>6.9444444444444458E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="4">
+        <v>16</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="5">
+        <v>4.26</v>
+      </c>
+      <c r="H20" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I20" s="5">
+        <v>279</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9583333333333332E-3</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" si="1"/>
+        <v>3.402777777777778E-3</v>
+      </c>
+      <c r="L20" s="24">
+        <f t="shared" si="2"/>
+        <v>3.2291666666666666E-3</v>
+      </c>
+      <c r="M20" s="24">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111136E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="4">
+        <v>17</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="5">
+        <v>4.29</v>
+      </c>
+      <c r="H21" s="5">
+        <v>4.93</v>
+      </c>
+      <c r="I21" s="5">
+        <v>281</v>
+      </c>
+      <c r="J21" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9791666666666669E-3</v>
+      </c>
+      <c r="K21" s="10">
+        <f t="shared" si="1"/>
+        <v>3.4236111111111108E-3</v>
+      </c>
+      <c r="L21" s="24">
+        <f t="shared" si="2"/>
+        <v>3.2523148148148147E-3</v>
+      </c>
+      <c r="M21" s="24">
+        <f t="shared" si="3"/>
+        <v>1.7129629629629613E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4">
+        <v>18</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="5">
+        <v>3.59</v>
+      </c>
+      <c r="H22" s="5">
+        <v>4.13</v>
+      </c>
+      <c r="I22" s="5">
+        <v>104</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4930555555555556E-3</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="1"/>
+        <v>2.8680555555555555E-3</v>
+      </c>
+      <c r="L22" s="24">
+        <f t="shared" si="2"/>
+        <v>1.2037037037037038E-3</v>
+      </c>
+      <c r="M22" s="24">
+        <f t="shared" si="3"/>
+        <v>1.6643518518518518E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="4">
+        <v>19</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="H23" s="5">
+        <v>2.76</v>
+      </c>
+      <c r="I23" s="5">
+        <v>154</v>
+      </c>
+      <c r="J23" s="10">
+        <f t="shared" si="0"/>
+        <v>1.6597222222222224E-3</v>
+      </c>
+      <c r="K23" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9166666666666666E-3</v>
+      </c>
+      <c r="L23" s="24">
+        <f t="shared" si="2"/>
+        <v>1.7824074074074075E-3</v>
+      </c>
+      <c r="M23" s="24">
+        <f t="shared" si="3"/>
+        <v>1.342592592592591E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="4">
+        <v>22</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="H24" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="I24" s="5">
+        <v>283</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8888888888888892E-3</v>
+      </c>
+      <c r="K24" s="10">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="L24" s="24">
+        <f t="shared" si="2"/>
+        <v>3.2754629629629631E-3</v>
+      </c>
+      <c r="M24" s="24">
+        <f t="shared" si="3"/>
+        <v>5.787037037037002E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="4">
+        <v>14</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="5">
+        <v>3.48</v>
+      </c>
+      <c r="H25" s="5">
+        <v>4</v>
+      </c>
+      <c r="I25" s="5">
+        <v>230</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4166666666666668E-3</v>
+      </c>
+      <c r="K25" s="10">
+        <f t="shared" si="1"/>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="L25" s="24">
+        <f t="shared" si="2"/>
+        <v>2.662037037037037E-3</v>
+      </c>
+      <c r="M25" s="24">
+        <f t="shared" si="3"/>
+        <v>1.1574074074074091E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="4">
+        <v>20</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="5">
+        <v>1.03</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I26" s="5">
+        <v>68</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="0"/>
+        <v>7.1527777777777779E-4</v>
+      </c>
+      <c r="K26" s="10">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333328E-4</v>
+      </c>
+      <c r="L26" s="24">
+        <f t="shared" si="2"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+      <c r="M26" s="24">
+        <f t="shared" si="3"/>
+        <v>4.6296296296296233E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="12"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="4">
+        <v>21</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I27" s="5">
+        <v>32</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" si="0"/>
+        <v>3.4027777777777778E-4</v>
+      </c>
+      <c r="K27" s="10">
+        <f t="shared" si="1"/>
+        <v>3.9583333333333332E-4</v>
+      </c>
+      <c r="L27" s="24">
+        <f t="shared" si="2"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="M27" s="24">
+        <f t="shared" si="3"/>
+        <v>2.5462962962962972E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027415B4991F41841B1A250D659A23981" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a6f577e764f505ffe57fae642640c87c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dbbedc70-ead9-41c7-bee8-2c47823ea795" xmlns:ns4="19b93533-c1e2-43ab-ab39-0c8609e457ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a7b2a257e9e5dd672313b72c10c8505" ns3:_="" ns4:_="">
+    <xsd:import namespace="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <xsd:import namespace="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dbbedc70-ead9-41c7-bee8-2c47823ea795" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="19b93533-c1e2-43ab-ab39-0c8609e457ac" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="13" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F668B66A-309C-4416-871D-514D51398915}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
+    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02750FF3-DF29-4E6A-8E82-4FDC91690270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D050E03-2C71-4FE4-8614-E510855E3A43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Se actualizan tiempos de operación y setup por elemento.
</commit_message>
<xml_diff>
--- a/SimulacionProceso/Tiempos por proceso.xlsx
+++ b/SimulacionProceso/Tiempos por proceso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/miarodriguezur_unal_edu_co/Documents/Doceabo semestre/AUTO/proyecto Auto/Proyecto_APM/SimulacionProceso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{0EE92507-21CF-4F82-8EBE-D3C7CE82A09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{4CA7F2C6-3765-4F42-B624-D8E8E0157753}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{0EE92507-21CF-4F82-8EBE-D3C7CE82A09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{645C3600-7087-48C3-8268-1349186AD4C7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C8728B57-2FEA-4814-B387-671D8068A2D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Corte</t>
   </si>
@@ -153,16 +153,31 @@
     <t>Tiempo Operativo + Setup (Minutos)</t>
   </si>
   <si>
-    <t>Tiempo Proceso (HH:MM:SS)</t>
-  </si>
-  <si>
     <t>Tiempo Operativo + Setup (HH:MM:SS)</t>
   </si>
   <si>
-    <t>Set-up time (HH:MM:SS)</t>
-  </si>
-  <si>
-    <t>Tiempo Proceso (Segundos)</t>
+    <t>Tiempo Proceso (HH:MM:SS) POR CICLA</t>
+  </si>
+  <si>
+    <t>Set-up time (HH:MM:SS)POR CICLA</t>
+  </si>
+  <si>
+    <t>Tiempo Proceso (HH:MM:SS) POR ELEMENTO</t>
+  </si>
+  <si>
+    <t>Set-up time (HH:MM:SS)POR ELEMENTO</t>
+  </si>
+  <si>
+    <t>Tiempo Proceso (Segundos) POR CICLA</t>
+  </si>
+  <si>
+    <t>Tiempo Proceso (Segundos) POR ELEMENTO</t>
+  </si>
+  <si>
+    <t>Tiempo Estandar (Minutos) POR CICLA</t>
+  </si>
+  <si>
+    <t>Tiempo Estandar (Segundos) POR ELEMENTO</t>
   </si>
 </sst>
 </file>
@@ -186,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +223,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +284,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -273,9 +312,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -284,21 +320,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,10 +669,10 @@
         <v>33</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="8" t="s">
         <v>38</v>
       </c>
@@ -660,19 +690,19 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="5">
         <v>3.75</v>
       </c>
@@ -693,15 +723,15 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="5">
         <v>4.12</v>
       </c>
@@ -722,15 +752,15 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="5">
         <v>1.2</v>
       </c>
@@ -751,12 +781,12 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="13">
+      <c r="B10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="21">
         <v>4</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -782,10 +812,10 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
@@ -809,10 +839,10 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -836,15 +866,15 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="5">
         <v>9.4</v>
       </c>
@@ -865,15 +895,15 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="5">
         <v>0.24</v>
       </c>
@@ -894,17 +924,17 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2">
         <v>7</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>1.97</v>
@@ -923,15 +953,15 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="2">
         <v>8</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5">
         <v>1.97</v>
@@ -950,15 +980,15 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="2">
         <v>9</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="5">
         <v>4.96</v>
       </c>
@@ -979,15 +1009,15 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="2">
         <v>10</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5">
         <v>1.97</v>
@@ -1006,19 +1036,19 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="4">
         <v>11</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="5">
         <v>0.44</v>
       </c>
@@ -1039,15 +1069,15 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="17"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="4">
         <v>12</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="5">
         <v>1.97</v>
       </c>
@@ -1068,15 +1098,15 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="4">
         <v>13</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="5">
         <v>1.26</v>
       </c>
@@ -1097,15 +1127,15 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="17"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="4">
         <v>15</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="5">
         <v>0.95</v>
       </c>
@@ -1126,15 +1156,15 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="4">
         <v>16</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="5">
         <v>4.26</v>
       </c>
@@ -1155,15 +1185,15 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="4">
         <v>17</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="5">
         <v>4.29</v>
       </c>
@@ -1184,17 +1214,17 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="20"/>
+      <c r="C25" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="4">
         <v>18</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="5">
         <v>3.59</v>
       </c>
@@ -1215,15 +1245,15 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="17"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="4">
         <v>19</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="5">
         <v>2.39</v>
       </c>
@@ -1244,15 +1274,15 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="4">
         <v>22</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="5">
         <v>4.16</v>
       </c>
@@ -1273,17 +1303,17 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4">
         <v>14</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="5">
         <v>3.48</v>
       </c>
@@ -1304,15 +1334,15 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="17"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="4">
         <v>20</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="5">
         <v>1.03</v>
       </c>
@@ -1333,15 +1363,15 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="4">
         <v>21</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="5">
         <v>0.49</v>
       </c>
@@ -1363,21 +1393,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="B7:B18"/>
     <mergeCell ref="B19:B30"/>
     <mergeCell ref="D10:D12"/>
@@ -1394,6 +1409,21 @@
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="C28:C30"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1401,64 +1431,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A6CFB2-59B8-49B2-A007-7D9BE44E8259}">
-  <dimension ref="B3:Q27"/>
+  <dimension ref="B3:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="Q3" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="5">
         <v>3.75</v>
       </c>
@@ -1468,34 +1511,48 @@
       <c r="I4" s="5">
         <v>60</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="K4" s="25">
+        <f>I4/12</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="10">
         <f>G4/1440</f>
         <v>2.6041666666666665E-3</v>
       </c>
-      <c r="K4" s="10">
+      <c r="M4" s="10">
         <f>H4/1440</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L4" s="24">
+      <c r="N4" s="15">
         <f>I4/86400</f>
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M4" s="24">
-        <f>K4-L4</f>
+      <c r="O4" s="15">
+        <f>M4-N4</f>
         <v>2.3055555555555555E-3</v>
       </c>
-      <c r="O4" s="20"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="16"/>
+      <c r="P4" s="29">
+        <f>K4/86400</f>
+        <v>5.7870370370370373E-5</v>
+      </c>
+      <c r="Q4" s="28">
+        <f>(J4-K4)/86400</f>
+        <v>1.9212962962962963E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="5">
         <v>4.12</v>
       </c>
@@ -1505,33 +1562,48 @@
       <c r="I5" s="5">
         <v>80</v>
       </c>
-      <c r="J5" s="10">
-        <f t="shared" ref="J5:J27" si="0">G5/1440</f>
+      <c r="J5" s="5">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="K5" s="5">
+        <f>I5/8</f>
+        <v>10</v>
+      </c>
+      <c r="L5" s="10">
+        <f>G5/1440</f>
         <v>2.8611111111111111E-3</v>
       </c>
-      <c r="K5" s="10">
-        <f t="shared" ref="K5:K27" si="1">H5/1440</f>
+      <c r="M5" s="10">
+        <f>H5/1440</f>
         <v>3.2986111111111111E-3</v>
       </c>
-      <c r="L5" s="24">
-        <f t="shared" ref="L5:L27" si="2">I5/86400</f>
+      <c r="N5" s="15">
+        <f>I5/86400</f>
         <v>9.2592592592592596E-4</v>
       </c>
-      <c r="M5" s="24">
-        <f t="shared" ref="M5:M27" si="3">K5-L5</f>
+      <c r="O5" s="15">
+        <f t="shared" ref="O5:O27" si="0">M5-N5</f>
         <v>2.3726851851851851E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="16"/>
+      <c r="P5" s="29">
+        <f t="shared" ref="P5:P27" si="1">K5/86400</f>
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="Q5" s="28">
+        <f t="shared" ref="Q5:Q9" si="2">(J5-K5)/86400</f>
+        <v>2.9652777777777777E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="5">
         <v>1.2</v>
       </c>
@@ -1541,30 +1613,45 @@
       <c r="I6" s="5">
         <v>24</v>
       </c>
-      <c r="J6" s="10">
-        <f t="shared" si="0"/>
+      <c r="J6" s="5">
+        <v>13.99</v>
+      </c>
+      <c r="K6" s="5">
+        <f>I6/6</f>
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
+        <f>G6/1440</f>
         <v>8.3333333333333328E-4</v>
       </c>
-      <c r="K6" s="10">
+      <c r="M6" s="10">
+        <f>H6/1440</f>
+        <v>9.7222222222222219E-4</v>
+      </c>
+      <c r="N6" s="15">
+        <f>I6/86400</f>
+        <v>2.7777777777777778E-4</v>
+      </c>
+      <c r="O6" s="15">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444436E-4</v>
+      </c>
+      <c r="P6" s="29">
         <f t="shared" si="1"/>
-        <v>9.7222222222222219E-4</v>
-      </c>
-      <c r="L6" s="24">
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="Q6" s="28">
         <f t="shared" si="2"/>
-        <v>2.7777777777777778E-4</v>
-      </c>
-      <c r="M6" s="24">
-        <f t="shared" si="3"/>
-        <v>6.9444444444444436E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="13">
+        <v>1.1562500000000001E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="21">
         <v>4</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1579,28 +1666,43 @@
       <c r="I7" s="5">
         <v>69</v>
       </c>
-      <c r="J7" s="10">
-        <f t="shared" si="0"/>
+      <c r="J7" s="5">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K7" s="25">
+        <f>I7/9</f>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="L7" s="10">
+        <f>G7/1440</f>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="K7" s="10">
+      <c r="M7" s="10">
+        <f>H7/1440</f>
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="N7" s="15">
+        <f>I7/86400</f>
+        <v>7.9861111111111116E-4</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.3263888888888891E-3</v>
+      </c>
+      <c r="P7" s="29">
         <f t="shared" si="1"/>
-        <v>2.1250000000000002E-3</v>
-      </c>
-      <c r="L7" s="24">
+        <v>8.8734567901234578E-5</v>
+      </c>
+      <c r="Q7" s="28">
         <f t="shared" si="2"/>
-        <v>7.9861111111111116E-4</v>
-      </c>
-      <c r="M7" s="24">
-        <f t="shared" si="3"/>
-        <v>1.3263888888888891E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
+        <v>1.473765432098765E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1613,28 +1715,43 @@
       <c r="I8" s="5">
         <v>35</v>
       </c>
-      <c r="J8" s="10">
-        <f t="shared" si="0"/>
+      <c r="J8" s="5">
+        <v>183.6</v>
+      </c>
+      <c r="K8" s="5">
+        <f>I8/1</f>
+        <v>35</v>
+      </c>
+      <c r="L8" s="10">
+        <f>G8/1440</f>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="K8" s="10">
+      <c r="M8" s="10">
+        <f>H8/1440</f>
+        <v>2.1250000000000002E-3</v>
+      </c>
+      <c r="N8" s="15">
+        <f>I8/86400</f>
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="O8" s="15">
+        <f t="shared" si="0"/>
+        <v>1.7199074074074076E-3</v>
+      </c>
+      <c r="P8" s="29">
         <f t="shared" si="1"/>
-        <v>2.1250000000000002E-3</v>
-      </c>
-      <c r="L8" s="24">
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="Q8" s="28">
         <f t="shared" si="2"/>
-        <v>4.0509259259259258E-4</v>
-      </c>
-      <c r="M8" s="24">
-        <f t="shared" si="3"/>
-        <v>1.7199074074074076E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
+        <v>1.7199074074074074E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1647,33 +1764,48 @@
       <c r="I9" s="5">
         <v>20</v>
       </c>
-      <c r="J9" s="10">
-        <f t="shared" si="0"/>
+      <c r="J9" s="5">
+        <v>45.9</v>
+      </c>
+      <c r="K9" s="5">
+        <f>I9/4</f>
+        <v>5</v>
+      </c>
+      <c r="L9" s="10">
+        <f>G9/1440</f>
         <v>1.8541666666666667E-3</v>
       </c>
-      <c r="K9" s="10">
-        <f t="shared" si="1"/>
+      <c r="M9" s="10">
+        <f>H9/1440</f>
         <v>2.1250000000000002E-3</v>
       </c>
-      <c r="L9" s="24">
+      <c r="N9" s="15">
+        <f>I9/86400</f>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="O9" s="15">
+        <f t="shared" si="0"/>
+        <v>1.8935185185185188E-3</v>
+      </c>
+      <c r="P9" s="29">
+        <f>K9/86400</f>
+        <v>5.7870370370370373E-5</v>
+      </c>
+      <c r="Q9" s="28">
         <f t="shared" si="2"/>
-        <v>2.3148148148148149E-4</v>
-      </c>
-      <c r="M9" s="24">
-        <f t="shared" si="3"/>
-        <v>1.8935185185185188E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="16"/>
+        <v>4.7337962962962964E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="5">
         <v>9.4</v>
       </c>
@@ -1683,33 +1815,49 @@
       <c r="I10" s="5">
         <v>300</v>
       </c>
-      <c r="J10" s="10">
-        <f t="shared" si="0"/>
+      <c r="J10" s="5">
+        <f>H10*60</f>
+        <v>648.6</v>
+      </c>
+      <c r="K10" s="5">
+        <f>I10</f>
+        <v>300</v>
+      </c>
+      <c r="L10" s="10">
+        <f>G10/1440</f>
         <v>6.5277777777777782E-3</v>
       </c>
-      <c r="K10" s="10">
-        <f t="shared" si="1"/>
+      <c r="M10" s="10">
+        <f>H10/1440</f>
         <v>7.5069444444444446E-3</v>
       </c>
-      <c r="L10" s="24">
-        <f t="shared" si="2"/>
+      <c r="N10" s="15">
+        <f>I10/86400</f>
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="M10" s="24">
-        <f t="shared" si="3"/>
+      <c r="O10" s="15">
+        <f t="shared" si="0"/>
         <v>4.0347222222222225E-3</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="16"/>
+      <c r="P10" s="29">
+        <f>N10</f>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="Q10" s="29">
+        <f>O10</f>
+        <v>4.0347222222222225E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="2">
         <v>6</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="5">
         <v>0.24</v>
       </c>
@@ -1719,35 +1867,51 @@
       <c r="I11" s="5">
         <v>4</v>
       </c>
-      <c r="J11" s="10">
-        <f t="shared" si="0"/>
+      <c r="J11" s="5">
+        <f t="shared" ref="J11:K27" si="3">H11*60</f>
+        <v>16.8</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" ref="K11:K27" si="4">I11</f>
+        <v>4</v>
+      </c>
+      <c r="L11" s="10">
+        <f>G11/1440</f>
         <v>1.6666666666666666E-4</v>
       </c>
-      <c r="K11" s="10">
-        <f t="shared" si="1"/>
+      <c r="M11" s="10">
+        <f>H11/1440</f>
         <v>1.9444444444444446E-4</v>
       </c>
-      <c r="L11" s="24">
-        <f t="shared" si="2"/>
+      <c r="N11" s="15">
+        <f>I11/86400</f>
         <v>4.6296296296296294E-5</v>
       </c>
-      <c r="M11" s="24">
-        <f t="shared" si="3"/>
+      <c r="O11" s="15">
+        <f t="shared" si="0"/>
         <v>1.4814814814814817E-4</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="16" t="s">
+      <c r="P11" s="29">
+        <f t="shared" ref="P11:P27" si="5">N11</f>
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="Q11" s="29">
+        <f t="shared" ref="Q11:Q27" si="6">O11</f>
+        <v>1.4814814814814817E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="19"/>
+      <c r="C12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>7</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
         <v>3.5</v>
@@ -1755,33 +1919,49 @@
       <c r="I12" s="5">
         <v>207</v>
       </c>
-      <c r="J12" s="10">
-        <f t="shared" si="0"/>
+      <c r="J12" s="5">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="4"/>
+        <v>207</v>
+      </c>
+      <c r="L12" s="10">
+        <f>G12/1440</f>
         <v>0</v>
       </c>
-      <c r="K12" s="10">
-        <f t="shared" si="1"/>
+      <c r="M12" s="10">
+        <f>H12/1440</f>
         <v>2.4305555555555556E-3</v>
       </c>
-      <c r="L12" s="24">
-        <f t="shared" si="2"/>
+      <c r="N12" s="15">
+        <f>I12/86400</f>
         <v>2.3958333333333331E-3</v>
       </c>
-      <c r="M12" s="24">
-        <f t="shared" si="3"/>
+      <c r="O12" s="15">
+        <f t="shared" si="0"/>
         <v>3.4722222222222446E-5</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="16"/>
+      <c r="P12" s="29">
+        <f t="shared" si="5"/>
+        <v>2.3958333333333331E-3</v>
+      </c>
+      <c r="Q12" s="29">
+        <f t="shared" si="6"/>
+        <v>3.4722222222222446E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="2">
         <v>8</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
         <v>1.21</v>
@@ -1789,33 +1969,49 @@
       <c r="I13" s="5">
         <v>71</v>
       </c>
-      <c r="J13" s="10">
-        <f t="shared" si="0"/>
+      <c r="J13" s="5">
+        <f t="shared" si="3"/>
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="L13" s="10">
+        <f>G13/1440</f>
         <v>0</v>
       </c>
-      <c r="K13" s="10">
-        <f t="shared" si="1"/>
+      <c r="M13" s="10">
+        <f>H13/1440</f>
         <v>8.4027777777777779E-4</v>
       </c>
-      <c r="L13" s="24">
-        <f t="shared" si="2"/>
+      <c r="N13" s="15">
+        <f>I13/86400</f>
         <v>8.2175925925925927E-4</v>
       </c>
-      <c r="M13" s="24">
-        <f t="shared" si="3"/>
+      <c r="O13" s="15">
+        <f t="shared" si="0"/>
         <v>1.8518518518518515E-5</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
+      <c r="P13" s="29">
+        <f t="shared" si="5"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="Q13" s="29">
+        <f t="shared" si="6"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="2">
         <v>9</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="5">
         <v>4.96</v>
       </c>
@@ -1825,33 +2021,49 @@
       <c r="I14" s="5">
         <v>270</v>
       </c>
-      <c r="J14" s="10">
-        <f t="shared" si="0"/>
+      <c r="J14" s="5">
+        <f t="shared" si="3"/>
+        <v>342</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="L14" s="10">
+        <f>G14/1440</f>
         <v>3.4444444444444444E-3</v>
       </c>
-      <c r="K14" s="10">
-        <f t="shared" si="1"/>
+      <c r="M14" s="10">
+        <f>H14/1440</f>
         <v>3.9583333333333337E-3</v>
       </c>
-      <c r="L14" s="24">
-        <f t="shared" si="2"/>
+      <c r="N14" s="15">
+        <f>I14/86400</f>
         <v>3.1250000000000002E-3</v>
       </c>
-      <c r="M14" s="24">
-        <f t="shared" si="3"/>
+      <c r="O14" s="15">
+        <f t="shared" si="0"/>
         <v>8.333333333333335E-4</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="16"/>
+      <c r="P14" s="29">
+        <f t="shared" si="5"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="Q14" s="29">
+        <f t="shared" si="6"/>
+        <v>8.333333333333335E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="2">
         <v>10</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>1.21</v>
@@ -1859,37 +2071,53 @@
       <c r="I15" s="5">
         <v>71</v>
       </c>
-      <c r="J15" s="10">
-        <f t="shared" si="0"/>
+      <c r="J15" s="5">
+        <f t="shared" si="3"/>
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="L15" s="10">
+        <f>G15/1440</f>
         <v>0</v>
       </c>
-      <c r="K15" s="10">
-        <f t="shared" si="1"/>
+      <c r="M15" s="10">
+        <f>H15/1440</f>
         <v>8.4027777777777779E-4</v>
       </c>
-      <c r="L15" s="24">
-        <f t="shared" si="2"/>
+      <c r="N15" s="15">
+        <f>I15/86400</f>
         <v>8.2175925925925927E-4</v>
       </c>
-      <c r="M15" s="24">
-        <f t="shared" si="3"/>
+      <c r="O15" s="15">
+        <f t="shared" si="0"/>
         <v>1.8518518518518515E-5</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="P15" s="29">
+        <f t="shared" si="5"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="Q15" s="29">
+        <f t="shared" si="6"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4">
         <v>11</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="5">
         <v>0.44</v>
       </c>
@@ -1899,36 +2127,51 @@
       <c r="I16" s="5">
         <v>20</v>
       </c>
-      <c r="J16" s="10">
-        <f t="shared" si="0"/>
+      <c r="J16" s="5">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="L16" s="10">
+        <f>G16/1440</f>
         <v>3.0555555555555555E-4</v>
       </c>
-      <c r="K16" s="10">
-        <f t="shared" si="1"/>
+      <c r="M16" s="10">
+        <f>H16/1440</f>
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="L16" s="24">
-        <f t="shared" si="2"/>
+      <c r="N16" s="15">
+        <f>I16/86400</f>
         <v>2.3148148148148149E-4</v>
       </c>
-      <c r="M16" s="24">
-        <f t="shared" si="3"/>
+      <c r="O16" s="15">
+        <f t="shared" si="0"/>
         <v>1.1574074074074075E-4</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="17"/>
+      <c r="P16" s="29">
+        <f t="shared" si="5"/>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="Q16" s="29">
+        <f t="shared" si="6"/>
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="4">
         <v>12</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="5">
         <v>1.97</v>
       </c>
@@ -1938,33 +2181,49 @@
       <c r="I17" s="5">
         <v>100</v>
       </c>
-      <c r="J17" s="10">
-        <f t="shared" si="0"/>
+      <c r="J17" s="5">
+        <f t="shared" si="3"/>
+        <v>135.6</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="L17" s="10">
+        <f>G17/1440</f>
         <v>1.3680555555555555E-3</v>
       </c>
-      <c r="K17" s="10">
-        <f t="shared" si="1"/>
+      <c r="M17" s="10">
+        <f>H17/1440</f>
         <v>1.5694444444444443E-3</v>
       </c>
-      <c r="L17" s="24">
-        <f t="shared" si="2"/>
+      <c r="N17" s="15">
+        <f>I17/86400</f>
         <v>1.1574074074074073E-3</v>
       </c>
-      <c r="M17" s="24">
-        <f t="shared" si="3"/>
+      <c r="O17" s="15">
+        <f t="shared" si="0"/>
         <v>4.1203703703703693E-4</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="17"/>
+      <c r="P17" s="29">
+        <f t="shared" si="5"/>
+        <v>1.1574074074074073E-3</v>
+      </c>
+      <c r="Q17" s="29">
+        <f t="shared" si="6"/>
+        <v>4.1203703703703693E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="20"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="4">
         <v>13</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="5">
         <v>1.26</v>
       </c>
@@ -1974,33 +2233,49 @@
       <c r="I18" s="5">
         <v>80</v>
       </c>
-      <c r="J18" s="10">
-        <f t="shared" si="0"/>
+      <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="L18" s="10">
+        <f>G18/1440</f>
         <v>8.7500000000000002E-4</v>
       </c>
-      <c r="K18" s="10">
-        <f t="shared" si="1"/>
+      <c r="M18" s="10">
+        <f>H18/1440</f>
         <v>1.0069444444444444E-3</v>
       </c>
-      <c r="L18" s="24">
-        <f t="shared" si="2"/>
+      <c r="N18" s="15">
+        <f>I18/86400</f>
         <v>9.2592592592592596E-4</v>
       </c>
-      <c r="M18" s="24">
-        <f t="shared" si="3"/>
+      <c r="O18" s="15">
+        <f t="shared" si="0"/>
         <v>8.1018518518518462E-5</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="17"/>
+      <c r="P18" s="29">
+        <f t="shared" si="5"/>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="Q18" s="29">
+        <f t="shared" si="6"/>
+        <v>8.1018518518518462E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="20"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="4">
         <v>15</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="5">
         <v>0.95</v>
       </c>
@@ -2010,33 +2285,49 @@
       <c r="I19" s="5">
         <v>60</v>
       </c>
-      <c r="J19" s="10">
-        <f t="shared" si="0"/>
+      <c r="J19" s="5">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="L19" s="10">
+        <f>G19/1440</f>
         <v>6.5972222222222224E-4</v>
       </c>
-      <c r="K19" s="10">
-        <f t="shared" si="1"/>
+      <c r="M19" s="10">
+        <f>H19/1440</f>
         <v>7.6388888888888893E-4</v>
       </c>
-      <c r="L19" s="24">
-        <f t="shared" si="2"/>
+      <c r="N19" s="15">
+        <f>I19/86400</f>
         <v>6.9444444444444447E-4</v>
       </c>
-      <c r="M19" s="24">
-        <f t="shared" si="3"/>
+      <c r="O19" s="15">
+        <f t="shared" si="0"/>
         <v>6.9444444444444458E-5</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="17"/>
+      <c r="P19" s="29">
+        <f t="shared" si="5"/>
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q19" s="29">
+        <f t="shared" si="6"/>
+        <v>6.9444444444444458E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="20"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="4">
         <v>16</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="5">
         <v>4.26</v>
       </c>
@@ -2046,33 +2337,49 @@
       <c r="I20" s="5">
         <v>279</v>
       </c>
-      <c r="J20" s="10">
-        <f t="shared" si="0"/>
+      <c r="J20" s="5">
+        <f t="shared" si="3"/>
+        <v>294</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="4"/>
+        <v>279</v>
+      </c>
+      <c r="L20" s="10">
+        <f>G20/1440</f>
         <v>2.9583333333333332E-3</v>
       </c>
-      <c r="K20" s="10">
-        <f t="shared" si="1"/>
+      <c r="M20" s="10">
+        <f>H20/1440</f>
         <v>3.402777777777778E-3</v>
       </c>
-      <c r="L20" s="24">
-        <f t="shared" si="2"/>
+      <c r="N20" s="15">
+        <f>I20/86400</f>
         <v>3.2291666666666666E-3</v>
       </c>
-      <c r="M20" s="24">
-        <f t="shared" si="3"/>
+      <c r="O20" s="15">
+        <f t="shared" si="0"/>
         <v>1.7361111111111136E-4</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="17"/>
+      <c r="P20" s="29">
+        <f t="shared" si="5"/>
+        <v>3.2291666666666666E-3</v>
+      </c>
+      <c r="Q20" s="29">
+        <f t="shared" si="6"/>
+        <v>1.7361111111111136E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="20"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="4">
         <v>17</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="5">
         <v>4.29</v>
       </c>
@@ -2082,35 +2389,51 @@
       <c r="I21" s="5">
         <v>281</v>
       </c>
-      <c r="J21" s="10">
-        <f t="shared" si="0"/>
+      <c r="J21" s="5">
+        <f t="shared" si="3"/>
+        <v>295.79999999999995</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="L21" s="10">
+        <f>G21/1440</f>
         <v>2.9791666666666669E-3</v>
       </c>
-      <c r="K21" s="10">
-        <f t="shared" si="1"/>
+      <c r="M21" s="10">
+        <f>H21/1440</f>
         <v>3.4236111111111108E-3</v>
       </c>
-      <c r="L21" s="24">
-        <f t="shared" si="2"/>
+      <c r="N21" s="15">
+        <f>I21/86400</f>
         <v>3.2523148148148147E-3</v>
       </c>
-      <c r="M21" s="24">
-        <f t="shared" si="3"/>
+      <c r="O21" s="15">
+        <f t="shared" si="0"/>
         <v>1.7129629629629613E-4</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="17" t="s">
+      <c r="P21" s="29">
+        <f t="shared" si="5"/>
+        <v>3.2523148148148147E-3</v>
+      </c>
+      <c r="Q21" s="29">
+        <f t="shared" si="6"/>
+        <v>1.7129629629629613E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="20"/>
+      <c r="C22" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="4">
         <v>18</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="5">
         <v>3.59</v>
       </c>
@@ -2120,33 +2443,49 @@
       <c r="I22" s="5">
         <v>104</v>
       </c>
-      <c r="J22" s="10">
-        <f t="shared" si="0"/>
+      <c r="J22" s="5">
+        <f t="shared" si="3"/>
+        <v>247.79999999999998</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="L22" s="10">
+        <f>G22/1440</f>
         <v>2.4930555555555556E-3</v>
       </c>
-      <c r="K22" s="10">
-        <f t="shared" si="1"/>
+      <c r="M22" s="10">
+        <f>H22/1440</f>
         <v>2.8680555555555555E-3</v>
       </c>
-      <c r="L22" s="24">
-        <f t="shared" si="2"/>
+      <c r="N22" s="15">
+        <f>I22/86400</f>
         <v>1.2037037037037038E-3</v>
       </c>
-      <c r="M22" s="24">
-        <f t="shared" si="3"/>
+      <c r="O22" s="15">
+        <f t="shared" si="0"/>
         <v>1.6643518518518518E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="17"/>
+      <c r="P22" s="29">
+        <f t="shared" si="5"/>
+        <v>1.2037037037037038E-3</v>
+      </c>
+      <c r="Q22" s="29">
+        <f t="shared" si="6"/>
+        <v>1.6643518518518518E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="20"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="4">
         <v>19</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="5">
         <v>2.39</v>
       </c>
@@ -2156,33 +2495,49 @@
       <c r="I23" s="5">
         <v>154</v>
       </c>
-      <c r="J23" s="10">
-        <f t="shared" si="0"/>
+      <c r="J23" s="5">
+        <f t="shared" si="3"/>
+        <v>165.6</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="L23" s="10">
+        <f>G23/1440</f>
         <v>1.6597222222222224E-3</v>
       </c>
-      <c r="K23" s="10">
-        <f t="shared" si="1"/>
+      <c r="M23" s="10">
+        <f>H23/1440</f>
         <v>1.9166666666666666E-3</v>
       </c>
-      <c r="L23" s="24">
-        <f t="shared" si="2"/>
+      <c r="N23" s="15">
+        <f>I23/86400</f>
         <v>1.7824074074074075E-3</v>
       </c>
-      <c r="M23" s="24">
-        <f t="shared" si="3"/>
+      <c r="O23" s="15">
+        <f t="shared" si="0"/>
         <v>1.342592592592591E-4</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="17"/>
+      <c r="P23" s="29">
+        <f t="shared" si="5"/>
+        <v>1.7824074074074075E-3</v>
+      </c>
+      <c r="Q23" s="29">
+        <f t="shared" si="6"/>
+        <v>1.342592592592591E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="4">
         <v>22</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="5">
         <v>4.16</v>
       </c>
@@ -2192,35 +2547,51 @@
       <c r="I24" s="5">
         <v>283</v>
       </c>
-      <c r="J24" s="10">
-        <f t="shared" si="0"/>
+      <c r="J24" s="5">
+        <f t="shared" si="3"/>
+        <v>288</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="4"/>
+        <v>283</v>
+      </c>
+      <c r="L24" s="10">
+        <f>G24/1440</f>
         <v>2.8888888888888892E-3</v>
       </c>
-      <c r="K24" s="10">
-        <f t="shared" si="1"/>
+      <c r="M24" s="10">
+        <f>H24/1440</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="L24" s="24">
-        <f t="shared" si="2"/>
+      <c r="N24" s="15">
+        <f>I24/86400</f>
         <v>3.2754629629629631E-3</v>
       </c>
-      <c r="M24" s="24">
-        <f t="shared" si="3"/>
+      <c r="O24" s="15">
+        <f t="shared" si="0"/>
         <v>5.787037037037002E-5</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="17" t="s">
+      <c r="P24" s="29">
+        <f t="shared" si="5"/>
+        <v>3.2754629629629631E-3</v>
+      </c>
+      <c r="Q24" s="29">
+        <f t="shared" si="6"/>
+        <v>5.787037037037002E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="20"/>
+      <c r="C25" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="4">
         <v>14</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="5">
         <v>3.48</v>
       </c>
@@ -2230,33 +2601,49 @@
       <c r="I25" s="5">
         <v>230</v>
       </c>
-      <c r="J25" s="10">
-        <f t="shared" si="0"/>
+      <c r="J25" s="5">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="L25" s="10">
+        <f>G25/1440</f>
         <v>2.4166666666666668E-3</v>
       </c>
-      <c r="K25" s="10">
-        <f t="shared" si="1"/>
+      <c r="M25" s="10">
+        <f>H25/1440</f>
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="L25" s="24">
-        <f t="shared" si="2"/>
+      <c r="N25" s="15">
+        <f>I25/86400</f>
         <v>2.662037037037037E-3</v>
       </c>
-      <c r="M25" s="24">
-        <f t="shared" si="3"/>
+      <c r="O25" s="15">
+        <f t="shared" si="0"/>
         <v>1.1574074074074091E-4</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="17"/>
+      <c r="P25" s="29">
+        <f t="shared" si="5"/>
+        <v>2.662037037037037E-3</v>
+      </c>
+      <c r="Q25" s="29">
+        <f t="shared" si="6"/>
+        <v>1.1574074074074091E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="20"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="4">
         <v>20</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="5">
         <v>1.03</v>
       </c>
@@ -2266,33 +2653,49 @@
       <c r="I26" s="5">
         <v>68</v>
       </c>
-      <c r="J26" s="10">
-        <f t="shared" si="0"/>
+      <c r="J26" s="5">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="L26" s="10">
+        <f>G26/1440</f>
         <v>7.1527777777777779E-4</v>
       </c>
-      <c r="K26" s="10">
-        <f t="shared" si="1"/>
+      <c r="M26" s="10">
+        <f>H26/1440</f>
         <v>8.3333333333333328E-4</v>
       </c>
-      <c r="L26" s="24">
-        <f t="shared" si="2"/>
+      <c r="N26" s="15">
+        <f>I26/86400</f>
         <v>7.8703703703703705E-4</v>
       </c>
-      <c r="M26" s="24">
-        <f t="shared" si="3"/>
+      <c r="O26" s="15">
+        <f t="shared" si="0"/>
         <v>4.6296296296296233E-5</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="17"/>
+      <c r="P26" s="29">
+        <f t="shared" si="5"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+      <c r="Q26" s="29">
+        <f t="shared" si="6"/>
+        <v>4.6296296296296233E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="20"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="4">
         <v>21</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="5">
         <v>0.49</v>
       </c>
@@ -2302,45 +2705,46 @@
       <c r="I27" s="5">
         <v>32</v>
       </c>
-      <c r="J27" s="10">
-        <f t="shared" si="0"/>
+      <c r="J27" s="5">
+        <f t="shared" si="3"/>
+        <v>34.199999999999996</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="L27" s="10">
+        <f>G27/1440</f>
         <v>3.4027777777777778E-4</v>
       </c>
-      <c r="K27" s="10">
-        <f t="shared" si="1"/>
+      <c r="M27" s="10">
+        <f>H27/1440</f>
         <v>3.9583333333333332E-4</v>
       </c>
-      <c r="L27" s="24">
-        <f t="shared" si="2"/>
+      <c r="N27" s="15">
+        <f>I27/86400</f>
         <v>3.7037037037037035E-4</v>
       </c>
-      <c r="M27" s="24">
-        <f t="shared" si="3"/>
+      <c r="O27" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5462962962962972E-5</v>
+      </c>
+      <c r="P27" s="29">
+        <f t="shared" si="5"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="Q27" s="29">
+        <f t="shared" si="6"/>
         <v>2.5462962962962972E-5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="B16:B27"/>
     <mergeCell ref="C16:C21"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
@@ -2352,6 +2756,21 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2359,21 +2778,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027415B4991F41841B1A250D659A23981" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a6f577e764f505ffe57fae642640c87c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dbbedc70-ead9-41c7-bee8-2c47823ea795" xmlns:ns4="19b93533-c1e2-43ab-ab39-0c8609e457ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a7b2a257e9e5dd672313b72c10c8505" ns3:_="" ns4:_="">
     <xsd:import namespace="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
@@ -2564,32 +2968,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F668B66A-309C-4416-871D-514D51398915}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
-    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02750FF3-DF29-4E6A-8E82-4FDC91690270}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D050E03-2C71-4FE4-8614-E510855E3A43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2606,4 +3000,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02750FF3-DF29-4E6A-8E82-4FDC91690270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F668B66A-309C-4416-871D-514D51398915}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
+    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Flujo operación completa para 1 cicla (Revisar setup de soldadura)
</commit_message>
<xml_diff>
--- a/SimulacionProceso/Tiempos por proceso.xlsx
+++ b/SimulacionProceso/Tiempos por proceso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/miarodriguezur_unal_edu_co/Documents/Doceabo semestre/AUTO/proyecto Auto/Proyecto_APM/SimulacionProceso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Github\Proyecto_APM\SimulacionProceso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{0EE92507-21CF-4F82-8EBE-D3C7CE82A09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{645C3600-7087-48C3-8268-1349186AD4C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD273906-4A53-49B9-AEAD-5E9FA515AC57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C8728B57-2FEA-4814-B387-671D8068A2D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C8728B57-2FEA-4814-B387-671D8068A2D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -293,15 +293,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="45" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -312,6 +312,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,15 +323,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="45" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,30 +650,30 @@
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="8" t="s">
         <v>38</v>
       </c>
@@ -689,20 +690,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="5">
         <v>3.75</v>
       </c>
@@ -722,16 +723,16 @@
         <v>3.9583333333333354E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="21"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="5">
         <v>4.12</v>
       </c>
@@ -751,16 +752,16 @@
         <v>4.3749999999999995E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="23"/>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="21"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="5">
         <v>1.2</v>
       </c>
@@ -780,13 +781,13 @@
         <v>1.3888888888888892E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="21">
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="23">
         <v>4</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -811,11 +812,11 @@
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="21"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
@@ -838,11 +839,11 @@
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="21"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="25"/>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
@@ -865,16 +866,16 @@
         <v>2.7083333333333343E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="23"/>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="21"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="5">
         <v>9.4</v>
       </c>
@@ -894,16 +895,16 @@
         <v>9.7916666666666638E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="23"/>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="5">
         <v>0.24</v>
       </c>
@@ -923,18 +924,18 @@
         <v>2.7777777777777799E-5</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="23" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="21"/>
+      <c r="C15" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2">
         <v>7</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>1.97</v>
@@ -952,16 +953,16 @@
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="23"/>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="21"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="2">
         <v>8</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5">
         <v>1.97</v>
@@ -979,16 +980,16 @@
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="23"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="21"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="2">
         <v>9</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="5">
         <v>4.96</v>
       </c>
@@ -1008,16 +1009,16 @@
         <v>5.1388888888888925E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="23"/>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="21"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="2">
         <v>10</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5">
         <v>1.97</v>
@@ -1035,20 +1036,20 @@
         <v>1.3680555555555555E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="4">
         <v>11</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="5">
         <v>0.44</v>
       </c>
@@ -1068,16 +1069,16 @@
         <v>4.1666666666666686E-5</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="24"/>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="4">
         <v>12</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="5">
         <v>1.97</v>
       </c>
@@ -1097,16 +1098,16 @@
         <v>2.0138888888888875E-4</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="24"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="4">
         <v>13</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="5">
         <v>1.26</v>
       </c>
@@ -1126,16 +1127,16 @@
         <v>1.3194444444444441E-4</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
-      <c r="C22" s="24"/>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="4">
         <v>15</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="5">
         <v>0.95</v>
       </c>
@@ -1155,16 +1156,16 @@
         <v>1.0416666666666669E-4</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="24"/>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="4">
         <v>16</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="5">
         <v>4.26</v>
       </c>
@@ -1184,16 +1185,16 @@
         <v>4.4444444444444479E-4</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="24"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="22"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="4">
         <v>17</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="5">
         <v>4.29</v>
       </c>
@@ -1213,18 +1214,18 @@
         <v>4.4444444444444392E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="24" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="22"/>
+      <c r="C25" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="4">
         <v>18</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="5">
         <v>3.59</v>
       </c>
@@ -1244,16 +1245,16 @@
         <v>3.749999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="24"/>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="4">
         <v>19</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="5">
         <v>2.39</v>
       </c>
@@ -1273,16 +1274,16 @@
         <v>2.5694444444444419E-4</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="24"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="22"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="4">
         <v>22</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="16"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="5">
         <v>4.16</v>
       </c>
@@ -1302,18 +1303,18 @@
         <v>4.4444444444444392E-4</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="24" t="s">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="22"/>
+      <c r="C28" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4">
         <v>14</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="16"/>
+      <c r="F28" s="28"/>
       <c r="G28" s="5">
         <v>3.48</v>
       </c>
@@ -1333,16 +1334,16 @@
         <v>3.6111111111111109E-4</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
-      <c r="C29" s="24"/>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="22"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="4">
         <v>20</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="16"/>
+      <c r="F29" s="28"/>
       <c r="G29" s="5">
         <v>1.03</v>
       </c>
@@ -1362,16 +1363,16 @@
         <v>1.1805555555555549E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="24"/>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="22"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="4">
         <v>21</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="16"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="5">
         <v>0.49</v>
       </c>
@@ -1393,6 +1394,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="B7:B18"/>
     <mergeCell ref="B19:B30"/>
     <mergeCell ref="D10:D12"/>
@@ -1409,21 +1425,6 @@
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="C28:C30"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1433,27 +1434,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A6CFB2-59B8-49B2-A007-7D9BE44E8259}">
   <dimension ref="B3:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="72" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="9" t="s">
         <v>38</v>
       </c>
@@ -1481,27 +1482,27 @@
       <c r="O3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="Q3" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="5">
         <v>3.75</v>
       </c>
@@ -1514,45 +1515,49 @@
       <c r="J4" s="5">
         <v>21.6</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="16">
         <f>I4/12</f>
         <v>5</v>
       </c>
       <c r="L4" s="10">
-        <f>G4/1440</f>
+        <f t="shared" ref="L4:L27" si="0">G4/1440</f>
         <v>2.6041666666666665E-3</v>
       </c>
       <c r="M4" s="10">
-        <f>H4/1440</f>
+        <f t="shared" ref="M4:M27" si="1">H4/1440</f>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="N4" s="15">
-        <f>I4/86400</f>
+        <f t="shared" ref="N4:N27" si="2">I4/86400</f>
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="O4" s="15">
         <f>M4-N4</f>
         <v>2.3055555555555555E-3</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="20">
         <f>K4/86400</f>
         <v>5.7870370370370373E-5</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="19">
         <f>(J4-K4)/86400</f>
         <v>1.9212962962962963E-4</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
+      <c r="R4" s="30">
+        <f>P4+Q4</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="21"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="5">
         <v>4.12</v>
       </c>
@@ -1570,40 +1575,44 @@
         <v>10</v>
       </c>
       <c r="L5" s="10">
-        <f>G5/1440</f>
+        <f t="shared" si="0"/>
         <v>2.8611111111111111E-3</v>
       </c>
       <c r="M5" s="10">
-        <f>H5/1440</f>
+        <f t="shared" si="1"/>
         <v>3.2986111111111111E-3</v>
       </c>
       <c r="N5" s="15">
-        <f>I5/86400</f>
+        <f t="shared" si="2"/>
         <v>9.2592592592592596E-4</v>
       </c>
       <c r="O5" s="15">
-        <f t="shared" ref="O5:O27" si="0">M5-N5</f>
+        <f t="shared" ref="O5:O27" si="3">M5-N5</f>
         <v>2.3726851851851851E-3</v>
       </c>
-      <c r="P5" s="29">
-        <f t="shared" ref="P5:P27" si="1">K5/86400</f>
+      <c r="P5" s="20">
+        <f t="shared" ref="P5:P8" si="4">K5/86400</f>
         <v>1.1574074074074075E-4</v>
       </c>
-      <c r="Q5" s="28">
-        <f t="shared" ref="Q5:Q9" si="2">(J5-K5)/86400</f>
+      <c r="Q5" s="19">
+        <f t="shared" ref="Q5:Q9" si="5">(J5-K5)/86400</f>
         <v>2.9652777777777777E-4</v>
       </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="23"/>
+      <c r="R5" s="30">
+        <f t="shared" ref="R5:R27" si="6">P5+Q5</f>
+        <v>4.1226851851851852E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="21"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="5">
         <v>1.2</v>
       </c>
@@ -1621,37 +1630,41 @@
         <v>4</v>
       </c>
       <c r="L6" s="10">
-        <f>G6/1440</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333328E-4</v>
       </c>
       <c r="M6" s="10">
-        <f>H6/1440</f>
+        <f t="shared" si="1"/>
         <v>9.7222222222222219E-4</v>
       </c>
       <c r="N6" s="15">
-        <f>I6/86400</f>
+        <f t="shared" si="2"/>
         <v>2.7777777777777778E-4</v>
       </c>
       <c r="O6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.9444444444444436E-4</v>
       </c>
-      <c r="P6" s="29">
-        <f t="shared" si="1"/>
+      <c r="P6" s="20">
+        <f t="shared" si="4"/>
         <v>4.6296296296296294E-5</v>
       </c>
-      <c r="Q6" s="28">
-        <f t="shared" si="2"/>
+      <c r="Q6" s="19">
+        <f t="shared" si="5"/>
         <v>1.1562500000000001E-4</v>
       </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="21">
+      <c r="R6" s="30">
+        <f t="shared" si="6"/>
+        <v>1.6192129629629629E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="21"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="23">
         <v>4</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1669,40 +1682,44 @@
       <c r="J7" s="5">
         <v>20.399999999999999</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="16">
         <f>I7/9</f>
         <v>7.666666666666667</v>
       </c>
       <c r="L7" s="10">
-        <f>G7/1440</f>
+        <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
       <c r="M7" s="10">
-        <f>H7/1440</f>
+        <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
       <c r="N7" s="15">
-        <f>I7/86400</f>
+        <f t="shared" si="2"/>
         <v>7.9861111111111116E-4</v>
       </c>
       <c r="O7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.3263888888888891E-3</v>
       </c>
-      <c r="P7" s="29">
-        <f t="shared" si="1"/>
+      <c r="P7" s="20">
+        <f t="shared" si="4"/>
         <v>8.8734567901234578E-5</v>
       </c>
-      <c r="Q7" s="28">
-        <f t="shared" si="2"/>
+      <c r="Q7" s="19">
+        <f t="shared" si="5"/>
         <v>1.473765432098765E-4</v>
       </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="R7" s="30">
+        <f t="shared" si="6"/>
+        <v>2.3611111111111109E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="21"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1723,35 +1740,39 @@
         <v>35</v>
       </c>
       <c r="L8" s="10">
-        <f>G8/1440</f>
+        <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
       <c r="M8" s="10">
-        <f>H8/1440</f>
+        <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
       <c r="N8" s="15">
-        <f>I8/86400</f>
+        <f t="shared" si="2"/>
         <v>4.0509259259259258E-4</v>
       </c>
       <c r="O8" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.7199074074074076E-3</v>
       </c>
-      <c r="P8" s="29">
-        <f t="shared" si="1"/>
+      <c r="P8" s="20">
+        <f t="shared" si="4"/>
         <v>4.0509259259259258E-4</v>
       </c>
-      <c r="Q8" s="28">
-        <f t="shared" si="2"/>
+      <c r="Q8" s="19">
+        <f t="shared" si="5"/>
         <v>1.7199074074074074E-3</v>
       </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="R8" s="30">
+        <f t="shared" si="6"/>
+        <v>2.1250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="21"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1772,40 +1793,44 @@
         <v>5</v>
       </c>
       <c r="L9" s="10">
-        <f>G9/1440</f>
+        <f t="shared" si="0"/>
         <v>1.8541666666666667E-3</v>
       </c>
       <c r="M9" s="10">
-        <f>H9/1440</f>
+        <f t="shared" si="1"/>
         <v>2.1250000000000002E-3</v>
       </c>
       <c r="N9" s="15">
-        <f>I9/86400</f>
+        <f t="shared" si="2"/>
         <v>2.3148148148148149E-4</v>
       </c>
       <c r="O9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.8935185185185188E-3</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9" s="20">
         <f>K9/86400</f>
         <v>5.7870370370370373E-5</v>
       </c>
-      <c r="Q9" s="28">
-        <f t="shared" si="2"/>
+      <c r="Q9" s="19">
+        <f t="shared" si="5"/>
         <v>4.7337962962962964E-4</v>
       </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
+      <c r="R9" s="30">
+        <f t="shared" si="6"/>
+        <v>5.3125000000000004E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="5">
         <v>9.4</v>
       </c>
@@ -1824,40 +1849,47 @@
         <v>300</v>
       </c>
       <c r="L10" s="10">
-        <f>G10/1440</f>
+        <f t="shared" si="0"/>
         <v>6.5277777777777782E-3</v>
       </c>
       <c r="M10" s="10">
-        <f>H10/1440</f>
+        <f t="shared" si="1"/>
         <v>7.5069444444444446E-3</v>
       </c>
       <c r="N10" s="15">
-        <f>I10/86400</f>
+        <f t="shared" si="2"/>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="O10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.0347222222222225E-3</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="20">
         <f>N10</f>
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="Q10" s="20">
         <f>O10</f>
         <v>4.0347222222222225E-3</v>
       </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="23"/>
+      <c r="R10" s="30">
+        <f t="shared" si="6"/>
+        <v>7.5069444444444446E-3</v>
+      </c>
+      <c r="S10" s="30">
+        <v>4.6990740740740743E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" s="21"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="2">
         <v>6</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="5">
         <v>0.24</v>
       </c>
@@ -1868,50 +1900,58 @@
         <v>4</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" ref="J11:K27" si="3">H11*60</f>
+        <f t="shared" ref="J11:J27" si="7">H11*60</f>
         <v>16.8</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" ref="K11:K27" si="4">I11</f>
+        <f t="shared" ref="K11:K27" si="8">I11</f>
         <v>4</v>
       </c>
       <c r="L11" s="10">
-        <f>G11/1440</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666666E-4</v>
       </c>
       <c r="M11" s="10">
-        <f>H11/1440</f>
+        <f t="shared" si="1"/>
         <v>1.9444444444444446E-4</v>
       </c>
       <c r="N11" s="15">
-        <f>I11/86400</f>
+        <f t="shared" si="2"/>
         <v>4.6296296296296294E-5</v>
       </c>
       <c r="O11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.4814814814814817E-4</v>
       </c>
-      <c r="P11" s="29">
-        <f t="shared" ref="P11:P27" si="5">N11</f>
+      <c r="P11" s="20">
+        <f t="shared" ref="P11:P27" si="9">N11</f>
         <v>4.6296296296296294E-5</v>
       </c>
-      <c r="Q11" s="29">
-        <f t="shared" ref="Q11:Q27" si="6">O11</f>
+      <c r="Q11" s="20">
+        <f t="shared" ref="Q11:Q27" si="10">O11</f>
         <v>1.4814814814814817E-4</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="23" t="s">
+      <c r="R11" s="30">
+        <f t="shared" si="6"/>
+        <v>1.9444444444444446E-4</v>
+      </c>
+      <c r="S11" s="30">
+        <f>S10+P10</f>
+        <v>8.1712962962962963E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="21"/>
+      <c r="C12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>7</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
         <v>3.5</v>
@@ -1920,48 +1960,56 @@
         <v>207</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="7"/>
+        <v>210</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="8"/>
+        <v>207</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.4305555555555556E-3</v>
+      </c>
+      <c r="N12" s="15">
+        <f t="shared" si="2"/>
+        <v>2.3958333333333331E-3</v>
+      </c>
+      <c r="O12" s="15">
         <f t="shared" si="3"/>
-        <v>210</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="4"/>
-        <v>207</v>
-      </c>
-      <c r="L12" s="10">
-        <f>G12/1440</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="10">
-        <f>H12/1440</f>
+        <v>3.4722222222222446E-5</v>
+      </c>
+      <c r="P12" s="20">
+        <f t="shared" si="9"/>
+        <v>2.3958333333333331E-3</v>
+      </c>
+      <c r="Q12" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4722222222222446E-5</v>
+      </c>
+      <c r="R12" s="30">
+        <f t="shared" si="6"/>
         <v>2.4305555555555556E-3</v>
       </c>
-      <c r="N12" s="15">
-        <f>I12/86400</f>
-        <v>2.3958333333333331E-3</v>
-      </c>
-      <c r="O12" s="15">
-        <f t="shared" si="0"/>
-        <v>3.4722222222222446E-5</v>
-      </c>
-      <c r="P12" s="29">
-        <f t="shared" si="5"/>
-        <v>2.3958333333333331E-3</v>
-      </c>
-      <c r="Q12" s="29">
-        <f t="shared" si="6"/>
-        <v>3.4722222222222446E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="23"/>
+      <c r="S12" s="30">
+        <f>S11+R12</f>
+        <v>1.0601851851851852E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="21"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="2">
         <v>8</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
         <v>1.21</v>
@@ -1970,48 +2018,56 @@
         <v>71</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="7"/>
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="1"/>
+        <v>8.4027777777777779E-4</v>
+      </c>
+      <c r="N13" s="15">
+        <f t="shared" si="2"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="O13" s="15">
         <f t="shared" si="3"/>
-        <v>72.599999999999994</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="L13" s="10">
-        <f>G13/1440</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <f>H13/1440</f>
+        <v>1.8518518518518515E-5</v>
+      </c>
+      <c r="P13" s="20">
+        <f t="shared" si="9"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="Q13" s="20">
+        <f t="shared" si="10"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+      <c r="R13" s="30">
+        <f t="shared" si="6"/>
         <v>8.4027777777777779E-4</v>
       </c>
-      <c r="N13" s="15">
-        <f>I13/86400</f>
-        <v>8.2175925925925927E-4</v>
-      </c>
-      <c r="O13" s="15">
-        <f t="shared" si="0"/>
-        <v>1.8518518518518515E-5</v>
-      </c>
-      <c r="P13" s="29">
-        <f t="shared" si="5"/>
-        <v>8.2175925925925927E-4</v>
-      </c>
-      <c r="Q13" s="29">
-        <f t="shared" si="6"/>
-        <v>1.8518518518518515E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="23"/>
+      <c r="S13" s="30">
+        <f>S12+R13</f>
+        <v>1.144212962962963E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="2">
         <v>9</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="5">
         <v>4.96</v>
       </c>
@@ -2022,48 +2078,56 @@
         <v>270</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="7"/>
+        <v>342</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="8"/>
+        <v>270</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="0"/>
+        <v>3.4444444444444444E-3</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="1"/>
+        <v>3.9583333333333337E-3</v>
+      </c>
+      <c r="N14" s="15">
+        <f t="shared" si="2"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="O14" s="15">
         <f t="shared" si="3"/>
-        <v>342</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-      <c r="L14" s="10">
-        <f>G14/1440</f>
-        <v>3.4444444444444444E-3</v>
-      </c>
-      <c r="M14" s="10">
-        <f>H14/1440</f>
+        <v>8.333333333333335E-4</v>
+      </c>
+      <c r="P14" s="20">
+        <f t="shared" si="9"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="Q14" s="20">
+        <f t="shared" si="10"/>
+        <v>8.333333333333335E-4</v>
+      </c>
+      <c r="R14" s="30">
+        <f t="shared" si="6"/>
         <v>3.9583333333333337E-3</v>
       </c>
-      <c r="N14" s="15">
-        <f>I14/86400</f>
-        <v>3.1250000000000002E-3</v>
-      </c>
-      <c r="O14" s="15">
-        <f t="shared" si="0"/>
-        <v>8.333333333333335E-4</v>
-      </c>
-      <c r="P14" s="29">
-        <f t="shared" si="5"/>
-        <v>3.1250000000000002E-3</v>
-      </c>
-      <c r="Q14" s="29">
-        <f t="shared" si="6"/>
-        <v>8.333333333333335E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="23"/>
+      <c r="S14" s="30">
+        <f>S13+R14</f>
+        <v>1.5400462962962963E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="21"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="2">
         <v>10</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>1.21</v>
@@ -2072,52 +2136,60 @@
         <v>71</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="7"/>
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="1"/>
+        <v>8.4027777777777779E-4</v>
+      </c>
+      <c r="N15" s="15">
+        <f t="shared" si="2"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="O15" s="15">
         <f t="shared" si="3"/>
-        <v>72.599999999999994</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="L15" s="10">
-        <f>G15/1440</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="10">
-        <f>H15/1440</f>
+        <v>1.8518518518518515E-5</v>
+      </c>
+      <c r="P15" s="20">
+        <f t="shared" si="9"/>
+        <v>8.2175925925925927E-4</v>
+      </c>
+      <c r="Q15" s="20">
+        <f t="shared" si="10"/>
+        <v>1.8518518518518515E-5</v>
+      </c>
+      <c r="R15" s="30">
+        <f t="shared" si="6"/>
         <v>8.4027777777777779E-4</v>
       </c>
-      <c r="N15" s="15">
-        <f>I15/86400</f>
-        <v>8.2175925925925927E-4</v>
-      </c>
-      <c r="O15" s="15">
-        <f t="shared" si="0"/>
-        <v>1.8518518518518515E-5</v>
-      </c>
-      <c r="P15" s="29">
-        <f t="shared" si="5"/>
-        <v>8.2175925925925927E-4</v>
-      </c>
-      <c r="Q15" s="29">
-        <f t="shared" si="6"/>
-        <v>1.8518518518518515E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="S15" s="30">
+        <f>S14+R15</f>
+        <v>1.624074074074074E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4">
         <v>11</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="5">
         <v>0.44</v>
       </c>
@@ -2128,50 +2200,56 @@
         <v>20</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="0"/>
+        <v>3.0555555555555555E-4</v>
+      </c>
+      <c r="M16" s="10">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="N16" s="15">
+        <f t="shared" si="2"/>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="O16" s="15">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="L16" s="10">
-        <f>G16/1440</f>
-        <v>3.0555555555555555E-4</v>
-      </c>
-      <c r="M16" s="10">
-        <f>H16/1440</f>
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="P16" s="20">
+        <f t="shared" si="9"/>
+        <v>2.3148148148148149E-4</v>
+      </c>
+      <c r="Q16" s="20">
+        <f t="shared" si="10"/>
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="R16" s="30">
+        <f t="shared" si="6"/>
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="N16" s="15">
-        <f>I16/86400</f>
-        <v>2.3148148148148149E-4</v>
-      </c>
-      <c r="O16" s="15">
-        <f t="shared" si="0"/>
-        <v>1.1574074074074075E-4</v>
-      </c>
-      <c r="P16" s="29">
-        <f t="shared" si="5"/>
-        <v>2.3148148148148149E-4</v>
-      </c>
-      <c r="Q16" s="29">
-        <f t="shared" si="6"/>
-        <v>1.1574074074074075E-4</v>
-      </c>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
-      <c r="C17" s="24"/>
+      <c r="S16" s="11">
+        <f>S15+R16</f>
+        <v>1.6587962962962961E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="4">
         <v>12</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="5">
         <v>1.97</v>
       </c>
@@ -2182,48 +2260,56 @@
         <v>100</v>
       </c>
       <c r="J17" s="5">
+        <f t="shared" si="7"/>
+        <v>135.6</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="0"/>
+        <v>1.3680555555555555E-3</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5694444444444443E-3</v>
+      </c>
+      <c r="N17" s="15">
+        <f t="shared" si="2"/>
+        <v>1.1574074074074073E-3</v>
+      </c>
+      <c r="O17" s="15">
         <f t="shared" si="3"/>
-        <v>135.6</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="L17" s="10">
-        <f>G17/1440</f>
-        <v>1.3680555555555555E-3</v>
-      </c>
-      <c r="M17" s="10">
-        <f>H17/1440</f>
+        <v>4.1203703703703693E-4</v>
+      </c>
+      <c r="P17" s="20">
+        <f t="shared" si="9"/>
+        <v>1.1574074074074073E-3</v>
+      </c>
+      <c r="Q17" s="20">
+        <f t="shared" si="10"/>
+        <v>4.1203703703703693E-4</v>
+      </c>
+      <c r="R17" s="30">
+        <f t="shared" si="6"/>
         <v>1.5694444444444443E-3</v>
       </c>
-      <c r="N17" s="15">
-        <f>I17/86400</f>
-        <v>1.1574074074074073E-3</v>
-      </c>
-      <c r="O17" s="15">
-        <f t="shared" si="0"/>
-        <v>4.1203703703703693E-4</v>
-      </c>
-      <c r="P17" s="29">
-        <f t="shared" si="5"/>
-        <v>1.1574074074074073E-3</v>
-      </c>
-      <c r="Q17" s="29">
-        <f t="shared" si="6"/>
-        <v>4.1203703703703693E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="24"/>
+      <c r="S17" s="11">
+        <f>S16+R17</f>
+        <v>1.8157407407407403E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="4">
         <v>13</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="5">
         <v>1.26</v>
       </c>
@@ -2234,48 +2320,56 @@
         <v>80</v>
       </c>
       <c r="J18" s="5">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="0"/>
+        <v>8.7500000000000002E-4</v>
+      </c>
+      <c r="M18" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0069444444444444E-3</v>
+      </c>
+      <c r="N18" s="15">
+        <f t="shared" si="2"/>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="O18" s="15">
         <f t="shared" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="L18" s="10">
-        <f>G18/1440</f>
-        <v>8.7500000000000002E-4</v>
-      </c>
-      <c r="M18" s="10">
-        <f>H18/1440</f>
+        <v>8.1018518518518462E-5</v>
+      </c>
+      <c r="P18" s="20">
+        <f t="shared" si="9"/>
+        <v>9.2592592592592596E-4</v>
+      </c>
+      <c r="Q18" s="20">
+        <f t="shared" si="10"/>
+        <v>8.1018518518518462E-5</v>
+      </c>
+      <c r="R18" s="30">
+        <f t="shared" si="6"/>
         <v>1.0069444444444444E-3</v>
       </c>
-      <c r="N18" s="15">
-        <f>I18/86400</f>
-        <v>9.2592592592592596E-4</v>
-      </c>
-      <c r="O18" s="15">
-        <f t="shared" si="0"/>
-        <v>8.1018518518518462E-5</v>
-      </c>
-      <c r="P18" s="29">
-        <f t="shared" si="5"/>
-        <v>9.2592592592592596E-4</v>
-      </c>
-      <c r="Q18" s="29">
-        <f t="shared" si="6"/>
-        <v>8.1018518518518462E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="24"/>
+      <c r="S18" s="11">
+        <f>S17+R18</f>
+        <v>1.9164351851851849E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="4">
         <v>15</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="5">
         <v>0.95</v>
       </c>
@@ -2286,48 +2380,56 @@
         <v>60</v>
       </c>
       <c r="J19" s="5">
+        <f t="shared" si="7"/>
+        <v>66</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="0"/>
+        <v>6.5972222222222224E-4</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" si="1"/>
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="N19" s="15">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="O19" s="15">
         <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="L19" s="10">
-        <f>G19/1440</f>
-        <v>6.5972222222222224E-4</v>
-      </c>
-      <c r="M19" s="10">
-        <f>H19/1440</f>
+        <v>6.9444444444444458E-5</v>
+      </c>
+      <c r="P19" s="20">
+        <f t="shared" si="9"/>
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q19" s="20">
+        <f t="shared" si="10"/>
+        <v>6.9444444444444458E-5</v>
+      </c>
+      <c r="R19" s="30">
+        <f t="shared" si="6"/>
         <v>7.6388888888888893E-4</v>
       </c>
-      <c r="N19" s="15">
-        <f>I19/86400</f>
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="O19" s="15">
-        <f t="shared" si="0"/>
-        <v>6.9444444444444458E-5</v>
-      </c>
-      <c r="P19" s="29">
-        <f t="shared" si="5"/>
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="Q19" s="29">
-        <f t="shared" si="6"/>
-        <v>6.9444444444444458E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="24"/>
+      <c r="S19" s="11">
+        <f>S18+R19</f>
+        <v>1.9928240740740739E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="4">
         <v>16</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="5">
         <v>4.26</v>
       </c>
@@ -2338,48 +2440,56 @@
         <v>279</v>
       </c>
       <c r="J20" s="5">
+        <f t="shared" si="7"/>
+        <v>294</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="8"/>
+        <v>279</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9583333333333332E-3</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="1"/>
+        <v>3.402777777777778E-3</v>
+      </c>
+      <c r="N20" s="15">
+        <f t="shared" si="2"/>
+        <v>3.2291666666666666E-3</v>
+      </c>
+      <c r="O20" s="15">
         <f t="shared" si="3"/>
-        <v>294</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="4"/>
-        <v>279</v>
-      </c>
-      <c r="L20" s="10">
-        <f>G20/1440</f>
-        <v>2.9583333333333332E-3</v>
-      </c>
-      <c r="M20" s="10">
-        <f>H20/1440</f>
+        <v>1.7361111111111136E-4</v>
+      </c>
+      <c r="P20" s="20">
+        <f t="shared" si="9"/>
+        <v>3.2291666666666666E-3</v>
+      </c>
+      <c r="Q20" s="20">
+        <f t="shared" si="10"/>
+        <v>1.7361111111111136E-4</v>
+      </c>
+      <c r="R20" s="30">
+        <f t="shared" si="6"/>
         <v>3.402777777777778E-3</v>
       </c>
-      <c r="N20" s="15">
-        <f>I20/86400</f>
-        <v>3.2291666666666666E-3</v>
-      </c>
-      <c r="O20" s="15">
-        <f t="shared" si="0"/>
-        <v>1.7361111111111136E-4</v>
-      </c>
-      <c r="P20" s="29">
-        <f t="shared" si="5"/>
-        <v>3.2291666666666666E-3</v>
-      </c>
-      <c r="Q20" s="29">
-        <f t="shared" si="6"/>
-        <v>1.7361111111111136E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="24"/>
+      <c r="S20" s="11">
+        <f>S19+R20</f>
+        <v>2.3331018518518518E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="4">
         <v>17</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="5">
         <v>4.29</v>
       </c>
@@ -2390,50 +2500,58 @@
         <v>281</v>
       </c>
       <c r="J21" s="5">
+        <f t="shared" si="7"/>
+        <v>295.79999999999995</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="8"/>
+        <v>281</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9791666666666669E-3</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="1"/>
+        <v>3.4236111111111108E-3</v>
+      </c>
+      <c r="N21" s="15">
+        <f t="shared" si="2"/>
+        <v>3.2523148148148147E-3</v>
+      </c>
+      <c r="O21" s="15">
         <f t="shared" si="3"/>
-        <v>295.79999999999995</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="4"/>
-        <v>281</v>
-      </c>
-      <c r="L21" s="10">
-        <f>G21/1440</f>
-        <v>2.9791666666666669E-3</v>
-      </c>
-      <c r="M21" s="10">
-        <f>H21/1440</f>
+        <v>1.7129629629629613E-4</v>
+      </c>
+      <c r="P21" s="20">
+        <f t="shared" si="9"/>
+        <v>3.2523148148148147E-3</v>
+      </c>
+      <c r="Q21" s="20">
+        <f t="shared" si="10"/>
+        <v>1.7129629629629613E-4</v>
+      </c>
+      <c r="R21" s="30">
+        <f t="shared" si="6"/>
         <v>3.4236111111111108E-3</v>
       </c>
-      <c r="N21" s="15">
-        <f>I21/86400</f>
-        <v>3.2523148148148147E-3</v>
-      </c>
-      <c r="O21" s="15">
-        <f t="shared" si="0"/>
-        <v>1.7129629629629613E-4</v>
-      </c>
-      <c r="P21" s="29">
-        <f t="shared" si="5"/>
-        <v>3.2523148148148147E-3</v>
-      </c>
-      <c r="Q21" s="29">
-        <f t="shared" si="6"/>
-        <v>1.7129629629629613E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
-      <c r="C22" s="24" t="s">
+      <c r="S21" s="11">
+        <f>S20+R21</f>
+        <v>2.6754629629629628E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="4">
         <v>18</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="5">
         <v>3.59</v>
       </c>
@@ -2444,48 +2562,52 @@
         <v>104</v>
       </c>
       <c r="J22" s="5">
+        <f t="shared" si="7"/>
+        <v>247.79999999999998</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="L22" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4930555555555556E-3</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="1"/>
+        <v>2.8680555555555555E-3</v>
+      </c>
+      <c r="N22" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2037037037037038E-3</v>
+      </c>
+      <c r="O22" s="15">
         <f t="shared" si="3"/>
-        <v>247.79999999999998</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="shared" si="4"/>
-        <v>104</v>
-      </c>
-      <c r="L22" s="10">
-        <f>G22/1440</f>
-        <v>2.4930555555555556E-3</v>
-      </c>
-      <c r="M22" s="10">
-        <f>H22/1440</f>
+        <v>1.6643518518518518E-3</v>
+      </c>
+      <c r="P22" s="20">
+        <f t="shared" si="9"/>
+        <v>1.2037037037037038E-3</v>
+      </c>
+      <c r="Q22" s="20">
+        <f t="shared" si="10"/>
+        <v>1.6643518518518518E-3</v>
+      </c>
+      <c r="R22" s="30">
+        <f t="shared" si="6"/>
         <v>2.8680555555555555E-3</v>
       </c>
-      <c r="N22" s="15">
-        <f>I22/86400</f>
-        <v>1.2037037037037038E-3</v>
-      </c>
-      <c r="O22" s="15">
-        <f t="shared" si="0"/>
-        <v>1.6643518518518518E-3</v>
-      </c>
-      <c r="P22" s="29">
-        <f t="shared" si="5"/>
-        <v>1.2037037037037038E-3</v>
-      </c>
-      <c r="Q22" s="29">
-        <f t="shared" si="6"/>
-        <v>1.6643518518518518E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="24"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="4">
         <v>19</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="5">
         <v>2.39</v>
       </c>
@@ -2496,48 +2618,52 @@
         <v>154</v>
       </c>
       <c r="J23" s="5">
+        <f t="shared" si="7"/>
+        <v>165.6</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="8"/>
+        <v>154</v>
+      </c>
+      <c r="L23" s="10">
+        <f t="shared" si="0"/>
+        <v>1.6597222222222224E-3</v>
+      </c>
+      <c r="M23" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9166666666666666E-3</v>
+      </c>
+      <c r="N23" s="15">
+        <f t="shared" si="2"/>
+        <v>1.7824074074074075E-3</v>
+      </c>
+      <c r="O23" s="15">
         <f t="shared" si="3"/>
-        <v>165.6</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" si="4"/>
-        <v>154</v>
-      </c>
-      <c r="L23" s="10">
-        <f>G23/1440</f>
-        <v>1.6597222222222224E-3</v>
-      </c>
-      <c r="M23" s="10">
-        <f>H23/1440</f>
+        <v>1.342592592592591E-4</v>
+      </c>
+      <c r="P23" s="20">
+        <f t="shared" si="9"/>
+        <v>1.7824074074074075E-3</v>
+      </c>
+      <c r="Q23" s="20">
+        <f t="shared" si="10"/>
+        <v>1.342592592592591E-4</v>
+      </c>
+      <c r="R23" s="30">
+        <f t="shared" si="6"/>
         <v>1.9166666666666666E-3</v>
       </c>
-      <c r="N23" s="15">
-        <f>I23/86400</f>
-        <v>1.7824074074074075E-3</v>
-      </c>
-      <c r="O23" s="15">
-        <f t="shared" si="0"/>
-        <v>1.342592592592591E-4</v>
-      </c>
-      <c r="P23" s="29">
-        <f t="shared" si="5"/>
-        <v>1.7824074074074075E-3</v>
-      </c>
-      <c r="Q23" s="29">
-        <f t="shared" si="6"/>
-        <v>1.342592592592591E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="24"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="22"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="4">
         <v>22</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="5">
         <v>4.16</v>
       </c>
@@ -2548,50 +2674,54 @@
         <v>283</v>
       </c>
       <c r="J24" s="5">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="8"/>
+        <v>283</v>
+      </c>
+      <c r="L24" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8888888888888892E-3</v>
+      </c>
+      <c r="M24" s="10">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="N24" s="15">
+        <f t="shared" si="2"/>
+        <v>3.2754629629629631E-3</v>
+      </c>
+      <c r="O24" s="15">
         <f t="shared" si="3"/>
-        <v>288</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" si="4"/>
-        <v>283</v>
-      </c>
-      <c r="L24" s="10">
-        <f>G24/1440</f>
-        <v>2.8888888888888892E-3</v>
-      </c>
-      <c r="M24" s="10">
-        <f>H24/1440</f>
+        <v>5.787037037037002E-5</v>
+      </c>
+      <c r="P24" s="20">
+        <f t="shared" si="9"/>
+        <v>3.2754629629629631E-3</v>
+      </c>
+      <c r="Q24" s="20">
+        <f t="shared" si="10"/>
+        <v>5.787037037037002E-5</v>
+      </c>
+      <c r="R24" s="30">
+        <f t="shared" si="6"/>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="N24" s="15">
-        <f>I24/86400</f>
-        <v>3.2754629629629631E-3</v>
-      </c>
-      <c r="O24" s="15">
-        <f t="shared" si="0"/>
-        <v>5.787037037037002E-5</v>
-      </c>
-      <c r="P24" s="29">
-        <f t="shared" si="5"/>
-        <v>3.2754629629629631E-3</v>
-      </c>
-      <c r="Q24" s="29">
-        <f t="shared" si="6"/>
-        <v>5.787037037037002E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="24" t="s">
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B25" s="22"/>
+      <c r="C25" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="4">
         <v>14</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="5">
         <v>3.48</v>
       </c>
@@ -2602,48 +2732,56 @@
         <v>230</v>
       </c>
       <c r="J25" s="5">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="8"/>
+        <v>230</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4166666666666668E-3</v>
+      </c>
+      <c r="M25" s="10">
+        <f t="shared" si="1"/>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="N25" s="15">
+        <f t="shared" si="2"/>
+        <v>2.662037037037037E-3</v>
+      </c>
+      <c r="O25" s="15">
         <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="K25" s="5">
-        <f t="shared" si="4"/>
-        <v>230</v>
-      </c>
-      <c r="L25" s="10">
-        <f>G25/1440</f>
-        <v>2.4166666666666668E-3</v>
-      </c>
-      <c r="M25" s="10">
-        <f>H25/1440</f>
+        <v>1.1574074074074091E-4</v>
+      </c>
+      <c r="P25" s="20">
+        <f t="shared" si="9"/>
+        <v>2.662037037037037E-3</v>
+      </c>
+      <c r="Q25" s="20">
+        <f t="shared" si="10"/>
+        <v>1.1574074074074091E-4</v>
+      </c>
+      <c r="R25" s="30">
+        <f t="shared" si="6"/>
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="N25" s="15">
-        <f>I25/86400</f>
-        <v>2.662037037037037E-3</v>
-      </c>
-      <c r="O25" s="15">
-        <f t="shared" si="0"/>
-        <v>1.1574074074074091E-4</v>
-      </c>
-      <c r="P25" s="29">
-        <f t="shared" si="5"/>
-        <v>2.662037037037037E-3</v>
-      </c>
-      <c r="Q25" s="29">
-        <f t="shared" si="6"/>
-        <v>1.1574074074074091E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="24"/>
+      <c r="S25" s="11">
+        <f>S21+R25</f>
+        <v>2.9532407407407407E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="4">
         <v>20</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="5">
         <v>1.03</v>
       </c>
@@ -2654,48 +2792,56 @@
         <v>68</v>
       </c>
       <c r="J26" s="5">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="0"/>
+        <v>7.1527777777777779E-4</v>
+      </c>
+      <c r="M26" s="10">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333328E-4</v>
+      </c>
+      <c r="N26" s="15">
+        <f t="shared" si="2"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+      <c r="O26" s="15">
         <f t="shared" si="3"/>
-        <v>72</v>
-      </c>
-      <c r="K26" s="5">
-        <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-      <c r="L26" s="10">
-        <f>G26/1440</f>
-        <v>7.1527777777777779E-4</v>
-      </c>
-      <c r="M26" s="10">
-        <f>H26/1440</f>
+        <v>4.6296296296296233E-5</v>
+      </c>
+      <c r="P26" s="20">
+        <f t="shared" si="9"/>
+        <v>7.8703703703703705E-4</v>
+      </c>
+      <c r="Q26" s="20">
+        <f t="shared" si="10"/>
+        <v>4.6296296296296233E-5</v>
+      </c>
+      <c r="R26" s="30">
+        <f t="shared" si="6"/>
         <v>8.3333333333333328E-4</v>
       </c>
-      <c r="N26" s="15">
-        <f>I26/86400</f>
-        <v>7.8703703703703705E-4</v>
-      </c>
-      <c r="O26" s="15">
-        <f t="shared" si="0"/>
-        <v>4.6296296296296233E-5</v>
-      </c>
-      <c r="P26" s="29">
-        <f t="shared" si="5"/>
-        <v>7.8703703703703705E-4</v>
-      </c>
-      <c r="Q26" s="29">
-        <f t="shared" si="6"/>
-        <v>4.6296296296296233E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="24"/>
+      <c r="S26" s="11">
+        <f>S25+R26</f>
+        <v>3.0365740740740738E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B27" s="22"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="4">
         <v>21</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="16"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="5">
         <v>0.49</v>
       </c>
@@ -2706,40 +2852,63 @@
         <v>32</v>
       </c>
       <c r="J27" s="5">
+        <f t="shared" si="7"/>
+        <v>34.199999999999996</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="8"/>
+        <v>32</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" si="0"/>
+        <v>3.4027777777777778E-4</v>
+      </c>
+      <c r="M27" s="10">
+        <f t="shared" si="1"/>
+        <v>3.9583333333333332E-4</v>
+      </c>
+      <c r="N27" s="15">
+        <f t="shared" si="2"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="O27" s="15">
         <f t="shared" si="3"/>
-        <v>34.199999999999996</v>
-      </c>
-      <c r="K27" s="5">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="L27" s="10">
-        <f>G27/1440</f>
-        <v>3.4027777777777778E-4</v>
-      </c>
-      <c r="M27" s="10">
-        <f>H27/1440</f>
+        <v>2.5462962962962972E-5</v>
+      </c>
+      <c r="P27" s="20">
+        <f t="shared" si="9"/>
+        <v>3.7037037037037035E-4</v>
+      </c>
+      <c r="Q27" s="20">
+        <f t="shared" si="10"/>
+        <v>2.5462962962962972E-5</v>
+      </c>
+      <c r="R27" s="30">
+        <f t="shared" si="6"/>
         <v>3.9583333333333332E-4</v>
       </c>
-      <c r="N27" s="15">
-        <f>I27/86400</f>
-        <v>3.7037037037037035E-4</v>
-      </c>
-      <c r="O27" s="15">
-        <f t="shared" si="0"/>
-        <v>2.5462962962962972E-5</v>
-      </c>
-      <c r="P27" s="29">
-        <f t="shared" si="5"/>
-        <v>3.7037037037037035E-4</v>
-      </c>
-      <c r="Q27" s="29">
-        <f t="shared" si="6"/>
-        <v>2.5462962962962972E-5</v>
+      <c r="S27" s="11">
+        <f>S26+R27</f>
+        <v>3.0761574074074073E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="B16:B27"/>
     <mergeCell ref="C16:C21"/>
     <mergeCell ref="E16:F16"/>
@@ -2756,21 +2925,6 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2778,6 +2932,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027415B4991F41841B1A250D659A23981" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a6f577e764f505ffe57fae642640c87c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dbbedc70-ead9-41c7-bee8-2c47823ea795" xmlns:ns4="19b93533-c1e2-43ab-ab39-0c8609e457ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a7b2a257e9e5dd672313b72c10c8505" ns3:_="" ns4:_="">
     <xsd:import namespace="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
@@ -2968,22 +3137,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F668B66A-309C-4416-871D-514D51398915}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
+    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02750FF3-DF29-4E6A-8E82-4FDC91690270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D050E03-2C71-4FE4-8614-E510855E3A43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3000,29 +3179,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02750FF3-DF29-4E6A-8E82-4FDC91690270}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F668B66A-309C-4416-871D-514D51398915}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="19b93533-c1e2-43ab-ab39-0c8609e457ac"/>
-    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>